<commit_message>
revised dataset names (thermal treatment)
</commit_message>
<xml_diff>
--- a/CaseStudy2_RoadDebris/EWU_Dashboard_InputTemplate_RoadDebris.xlsx
+++ b/CaseStudy2_RoadDebris/EWU_Dashboard_InputTemplate_RoadDebris.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\CaseStudy3_RoadDebris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F403FC6-F00E-4CA0-931F-6D37BC41D921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8A5FF2-0BB0-41D3-87C7-5EE15AD1DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="452">
   <si>
     <t>input</t>
   </si>
@@ -2438,12 +2438,6 @@
     <t>#C00000</t>
   </si>
   <si>
-    <t>Kaja Mol, David Laner &amp; Sarah Schmidt</t>
-  </si>
-  <si>
-    <t>EWU_RoadDebris</t>
-  </si>
-  <si>
     <t>Road debris</t>
   </si>
   <si>
@@ -2472,9 +2466,6 @@
     <t>TP1</t>
   </si>
   <si>
-    <t>treatment of road debris, incineration, treatment path</t>
-  </si>
-  <si>
     <t>Assumption</t>
   </si>
   <si>
@@ -2493,9 +2484,6 @@
     <t>TP1_road_debris</t>
   </si>
   <si>
-    <t>treatment of road debris, incineration, treatment path road debris</t>
-  </si>
-  <si>
     <t>TP2_road_debris</t>
   </si>
   <si>
@@ -2506,12 +2494,6 @@
   </si>
   <si>
     <t>treatment of road debris, disposal on landfills, treatment path road debris</t>
-  </si>
-  <si>
-    <t>Incineration-REKOI</t>
-  </si>
-  <si>
-    <t>treatment of road debris, incineration, REKOI</t>
   </si>
   <si>
     <t>Incineration</t>
@@ -2522,12 +2504,6 @@
 Säuberli E.</t>
   </si>
   <si>
-    <t>Incineration-REKOII</t>
-  </si>
-  <si>
-    <t>treatment of road debris, incineration, REKOII</t>
-  </si>
-  <si>
     <t>LandfillConstruction</t>
   </si>
   <si>
@@ -2773,6 +2749,33 @@
   </si>
   <si>
     <t>Weighting factors are used to aggregate impact category wise calculated impacts and indicator scores.</t>
+  </si>
+  <si>
+    <t>ThermalTreatment-REKOI</t>
+  </si>
+  <si>
+    <t>ThermalTreatment-REKOII</t>
+  </si>
+  <si>
+    <t>treatment of road debris, thermal treatment, treatment path</t>
+  </si>
+  <si>
+    <t>treatment of road debris, thermal treatment, treatment path road debris</t>
+  </si>
+  <si>
+    <t>treatment of road debris, thermal treatment, REKOI</t>
+  </si>
+  <si>
+    <t>treatment of road debris, thermal treatment, REKOII</t>
+  </si>
+  <si>
+    <t>Thermal Treatment</t>
+  </si>
+  <si>
+    <t>EWU_RoadDebris_v2</t>
+  </si>
+  <si>
+    <t>Sarah Schmidt, David Laner &amp; Kaja Mol</t>
   </si>
 </sst>
 </file>
@@ -4686,7 +4689,7 @@
     </row>
     <row r="4" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="78" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B4" s="78"/>
     </row>
@@ -4702,7 +4705,7 @@
     </row>
     <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="77" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B7" s="76"/>
     </row>
@@ -5275,19 +5278,19 @@
     <row r="1" spans="1:27" ht="91" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="23" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>200</v>
@@ -6564,7 +6567,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B2" s="74" t="s">
         <v>335</v>
@@ -6572,7 +6575,7 @@
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B3" s="74" t="s">
         <v>339</v>
@@ -6580,7 +6583,7 @@
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B4" s="74" t="s">
         <v>337</v>
@@ -6588,7 +6591,7 @@
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B5" s="74" t="s">
         <v>176</v>
@@ -6596,31 +6599,31 @@
     </row>
     <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B9" s="74" t="s">
         <v>336</v>
@@ -6631,7 +6634,7 @@
         <v>338</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -6728,7 +6731,7 @@
     </row>
     <row r="4" spans="1:11" s="28" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="78" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="26"/>
@@ -6775,7 +6778,7 @@
     </row>
     <row r="7" spans="1:11" s="28" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="77" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B7" s="76"/>
       <c r="C7" s="26"/>
@@ -7148,7 +7151,7 @@
         <v>222</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7204,7 +7207,7 @@
         <v>237</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28" x14ac:dyDescent="0.3">
@@ -7260,7 +7263,7 @@
         <v>239</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -7276,7 +7279,7 @@
         <v>183</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -7294,7 +7297,7 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7344,7 +7347,7 @@
         <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>341</v>
+        <v>450</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>66</v>
@@ -7373,7 +7376,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>340</v>
+        <v>451</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="53" t="s">
@@ -7425,7 +7428,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -7433,7 +7436,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -7441,7 +7444,7 @@
         <v>166</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.3">
@@ -7606,8 +7609,8 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7662,10 +7665,10 @@
     </row>
     <row r="2" spans="1:11" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>8</v>
@@ -7679,10 +7682,10 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K2" s="58" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7690,7 +7693,7 @@
         <v>334</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
@@ -7702,22 +7705,22 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K3" s="58" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>351</v>
+        <v>445</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>8</v>
@@ -7728,23 +7731,23 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K4" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>8</v>
@@ -7755,23 +7758,23 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K5" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>8</v>
@@ -7782,23 +7785,23 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K6" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>8</v>
@@ -7808,24 +7811,24 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K7" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>8</v>
@@ -7835,24 +7838,24 @@
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K8" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>8</v>
@@ -7862,24 +7865,24 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K9" s="59" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -7888,25 +7891,25 @@
         <v>14</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>365</v>
+        <v>449</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K10" s="58" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>8</v>
@@ -7915,25 +7918,25 @@
         <v>14</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>365</v>
+        <v>449</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K11" s="58" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -7942,25 +7945,25 @@
         <v>14</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K12" s="58" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -7969,24 +7972,24 @@
         <v>14</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K13" s="58" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>13</v>
@@ -7995,7 +7998,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -8003,15 +8006,15 @@
       <c r="I14" s="9"/>
       <c r="J14" s="58"/>
       <c r="K14" s="58" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>13</v>
@@ -8020,7 +8023,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -8028,15 +8031,15 @@
       <c r="I15" s="9"/>
       <c r="J15" s="58"/>
       <c r="K15" s="58" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>13</v>
@@ -8045,7 +8048,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -8053,15 +8056,15 @@
       <c r="I16" s="9"/>
       <c r="J16" s="60"/>
       <c r="K16" s="58" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="57" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>8</v>
@@ -8081,10 +8084,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>8</v>
@@ -8104,16 +8107,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -8127,16 +8130,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -8150,16 +8153,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -8173,16 +8176,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -8196,10 +8199,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>8</v>
@@ -8219,10 +8222,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>8</v>
@@ -8256,7 +8259,7 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -8306,10 +8309,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C2" s="61" t="s">
         <v>8</v>
@@ -8318,10 +8321,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F2" s="61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G2" s="61" t="s">
         <v>9</v>
@@ -8336,22 +8339,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="61" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C3" s="61" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G3" s="61" t="s">
         <v>9</v>
@@ -8366,10 +8369,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C4" s="61" t="s">
         <v>8</v>
@@ -8378,10 +8381,10 @@
         <v>15</v>
       </c>
       <c r="E4" s="61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F4" s="61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G4" s="61" t="s">
         <v>9</v>
@@ -8396,22 +8399,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C5" s="61" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G5" s="61" t="s">
         <v>9</v>
@@ -8426,7 +8429,7 @@
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B6" s="62" t="s">
         <v>334</v>
@@ -8438,7 +8441,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F6" s="62" t="s">
         <v>334</v>
@@ -8456,10 +8459,10 @@
     </row>
     <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
-        <v>351</v>
+        <v>445</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C7" s="62" t="s">
         <v>8</v>
@@ -8468,7 +8471,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>334</v>
@@ -8487,10 +8490,10 @@
     </row>
     <row r="8" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C8" s="62" t="s">
         <v>8</v>
@@ -8499,7 +8502,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F8" s="62" t="s">
         <v>334</v>
@@ -8518,10 +8521,10 @@
     </row>
     <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C9" s="62" t="s">
         <v>8</v>
@@ -8530,7 +8533,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F9" s="62" t="s">
         <v>334</v>
@@ -8549,10 +8552,10 @@
     </row>
     <row r="10" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="63" t="s">
-        <v>351</v>
+        <v>445</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C10" s="63" t="s">
         <v>8</v>
@@ -8561,10 +8564,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>351</v>
+        <v>445</v>
       </c>
       <c r="F10" s="63" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G10" s="63" t="s">
         <v>9</v>
@@ -8579,10 +8582,10 @@
     </row>
     <row r="11" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="63" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C11" s="63" t="s">
         <v>8</v>
@@ -8591,10 +8594,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>351</v>
+        <v>445</v>
       </c>
       <c r="F11" s="63" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G11" s="63" t="s">
         <v>9</v>
@@ -8609,10 +8612,10 @@
     </row>
     <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>8</v>
@@ -8621,10 +8624,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G12" s="64" t="s">
         <v>9</v>
@@ -8639,10 +8642,10 @@
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="64" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C13" s="64" t="s">
         <v>8</v>
@@ -8651,10 +8654,10 @@
         <v>9</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G13" s="64" t="s">
         <v>9</v>
@@ -8669,10 +8672,10 @@
     </row>
     <row r="14" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C14" s="65" t="s">
         <v>8</v>
@@ -8681,10 +8684,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G14" s="65" t="s">
         <v>9</v>
@@ -8699,10 +8702,10 @@
     </row>
     <row r="15" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="65" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>8</v>
@@ -8711,10 +8714,10 @@
         <v>9</v>
       </c>
       <c r="E15" s="65" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F15" s="65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G15" s="65" t="s">
         <v>9</v>
@@ -8729,10 +8732,10 @@
     </row>
     <row r="16" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="66" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C16" s="66" t="s">
         <v>8</v>
@@ -8741,10 +8744,10 @@
         <v>9</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G16" s="66" t="s">
         <v>9</v>
@@ -8759,10 +8762,10 @@
     </row>
     <row r="17" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="66" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="C17" s="66" t="s">
         <v>8</v>
@@ -8771,10 +8774,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="66" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G17" s="66" t="s">
         <v>9</v>
@@ -8789,10 +8792,10 @@
     </row>
     <row r="18" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="66" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="C18" s="66" t="s">
         <v>8</v>
@@ -8801,10 +8804,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>358</v>
+        <v>446</v>
       </c>
       <c r="F18" s="66" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G18" s="66" t="s">
         <v>9</v>
@@ -8819,10 +8822,10 @@
     </row>
     <row r="19" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="67" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C19" s="67" t="s">
         <v>8</v>
@@ -8831,10 +8834,10 @@
         <v>9</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G19" s="67" t="s">
         <v>9</v>
@@ -8849,10 +8852,10 @@
     </row>
     <row r="20" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="67" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C20" s="67" t="s">
         <v>8</v>
@@ -8861,10 +8864,10 @@
         <v>14</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F20" s="67" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G20" s="67" t="s">
         <v>9</v>
@@ -8879,10 +8882,10 @@
     </row>
     <row r="21" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="68" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C21" s="68" t="s">
         <v>8</v>
@@ -8891,10 +8894,10 @@
         <v>9</v>
       </c>
       <c r="E21" s="68" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F21" s="68" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G21" s="68" t="s">
         <v>9</v>
@@ -8909,10 +8912,10 @@
     </row>
     <row r="22" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="68" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C22" s="68" t="s">
         <v>8</v>
@@ -8921,10 +8924,10 @@
         <v>14</v>
       </c>
       <c r="E22" s="68" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F22" s="68" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G22" s="68" t="s">
         <v>9</v>
@@ -8939,10 +8942,10 @@
     </row>
     <row r="23" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="C23" s="69" t="s">
         <v>8</v>
@@ -8951,10 +8954,10 @@
         <v>14</v>
       </c>
       <c r="E23" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>14</v>
@@ -8969,10 +8972,10 @@
     </row>
     <row r="24" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="69" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C24" s="69" t="s">
         <v>13</v>
@@ -8981,10 +8984,10 @@
         <v>16</v>
       </c>
       <c r="E24" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G24" s="69" t="s">
         <v>14</v>
@@ -9000,10 +9003,10 @@
     </row>
     <row r="25" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="69" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C25" s="69" t="s">
         <v>13</v>
@@ -9012,10 +9015,10 @@
         <v>9</v>
       </c>
       <c r="E25" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F25" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G25" s="69" t="s">
         <v>14</v>
@@ -9030,10 +9033,10 @@
     </row>
     <row r="26" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="69" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C26" s="69" t="s">
         <v>13</v>
@@ -9042,10 +9045,10 @@
         <v>16</v>
       </c>
       <c r="E26" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F26" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G26" s="69" t="s">
         <v>14</v>
@@ -9061,10 +9064,10 @@
     </row>
     <row r="27" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="69" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C27" s="69" t="s">
         <v>8</v>
@@ -9073,10 +9076,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F27" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G27" s="69" t="s">
         <v>14</v>
@@ -9091,22 +9094,22 @@
     </row>
     <row r="28" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="69" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C28" s="69" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="69" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E28" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G28" s="69" t="s">
         <v>14</v>
@@ -9121,10 +9124,10 @@
     </row>
     <row r="29" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="69" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C29" s="69" t="s">
         <v>8</v>
@@ -9133,10 +9136,10 @@
         <v>12</v>
       </c>
       <c r="E29" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F29" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G29" s="69" t="s">
         <v>14</v>
@@ -9151,10 +9154,10 @@
     </row>
     <row r="30" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="69" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C30" s="69" t="s">
         <v>8</v>
@@ -9163,10 +9166,10 @@
         <v>12</v>
       </c>
       <c r="E30" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F30" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G30" s="69" t="s">
         <v>14</v>
@@ -9181,22 +9184,22 @@
     </row>
     <row r="31" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="69" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="69" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E31" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>14</v>
@@ -9211,22 +9214,22 @@
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="69" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C32" s="69" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G32" s="69" t="s">
         <v>14</v>
@@ -9241,22 +9244,22 @@
     </row>
     <row r="33" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="69" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C33" s="69" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F33" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G33" s="69" t="s">
         <v>14</v>
@@ -9271,22 +9274,22 @@
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="69" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C34" s="69" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E34" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G34" s="69" t="s">
         <v>14</v>
@@ -9301,10 +9304,10 @@
     </row>
     <row r="35" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="69" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C35" s="69" t="s">
         <v>8</v>
@@ -9313,10 +9316,10 @@
         <v>14</v>
       </c>
       <c r="E35" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G35" s="69" t="s">
         <v>14</v>
@@ -9331,10 +9334,10 @@
     </row>
     <row r="36" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="69" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C36" s="69" t="s">
         <v>8</v>
@@ -9343,10 +9346,10 @@
         <v>16</v>
       </c>
       <c r="E36" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F36" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G36" s="69" t="s">
         <v>14</v>
@@ -9361,10 +9364,10 @@
     </row>
     <row r="37" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="69" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C37" s="69" t="s">
         <v>8</v>
@@ -9373,10 +9376,10 @@
         <v>16</v>
       </c>
       <c r="E37" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F37" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G37" s="69" t="s">
         <v>14</v>
@@ -9391,10 +9394,10 @@
     </row>
     <row r="38" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="69" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C38" s="69" t="s">
         <v>8</v>
@@ -9403,10 +9406,10 @@
         <v>15</v>
       </c>
       <c r="E38" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F38" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G38" s="69" t="s">
         <v>14</v>
@@ -9421,10 +9424,10 @@
     </row>
     <row r="39" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="69" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C39" s="69" t="s">
         <v>8</v>
@@ -9433,10 +9436,10 @@
         <v>16</v>
       </c>
       <c r="E39" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F39" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G39" s="69" t="s">
         <v>14</v>
@@ -9451,22 +9454,22 @@
     </row>
     <row r="40" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="69" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B40" s="69" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C40" s="69" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="69" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E40" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F40" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G40" s="69" t="s">
         <v>14</v>
@@ -9481,22 +9484,22 @@
     </row>
     <row r="41" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="69" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B41" s="69" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C41" s="69" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="69" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E41" s="69" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="F41" s="69" t="s">
-        <v>363</v>
+        <v>443</v>
       </c>
       <c r="G41" s="69" t="s">
         <v>14</v>
@@ -9511,10 +9514,10 @@
     </row>
     <row r="42" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="B42" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="C42" s="70" t="s">
         <v>8</v>
@@ -9523,10 +9526,10 @@
         <v>14</v>
       </c>
       <c r="E42" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F42" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G42" s="70" t="s">
         <v>14</v>
@@ -9541,10 +9544,10 @@
     </row>
     <row r="43" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="70" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B43" s="70" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C43" s="70" t="s">
         <v>13</v>
@@ -9553,10 +9556,10 @@
         <v>16</v>
       </c>
       <c r="E43" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F43" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G43" s="70" t="s">
         <v>14</v>
@@ -9572,10 +9575,10 @@
     </row>
     <row r="44" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="70" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B44" s="70" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C44" s="70" t="s">
         <v>13</v>
@@ -9584,10 +9587,10 @@
         <v>9</v>
       </c>
       <c r="E44" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F44" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G44" s="70" t="s">
         <v>14</v>
@@ -9602,10 +9605,10 @@
     </row>
     <row r="45" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="70" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B45" s="70" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C45" s="70" t="s">
         <v>13</v>
@@ -9614,10 +9617,10 @@
         <v>16</v>
       </c>
       <c r="E45" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F45" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G45" s="70" t="s">
         <v>14</v>
@@ -9633,10 +9636,10 @@
     </row>
     <row r="46" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="70" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C46" s="70" t="s">
         <v>8</v>
@@ -9645,10 +9648,10 @@
         <v>16</v>
       </c>
       <c r="E46" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F46" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G46" s="70" t="s">
         <v>14</v>
@@ -9663,22 +9666,22 @@
     </row>
     <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="70" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C47" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="70" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E47" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F47" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G47" s="70" t="s">
         <v>14</v>
@@ -9693,10 +9696,10 @@
     </row>
     <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="70" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B48" s="70" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C48" s="70" t="s">
         <v>8</v>
@@ -9705,10 +9708,10 @@
         <v>12</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F48" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G48" s="70" t="s">
         <v>14</v>
@@ -9723,10 +9726,10 @@
     </row>
     <row r="49" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="70" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B49" s="70" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C49" s="70" t="s">
         <v>8</v>
@@ -9735,10 +9738,10 @@
         <v>12</v>
       </c>
       <c r="E49" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F49" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G49" s="70" t="s">
         <v>14</v>
@@ -9753,22 +9756,22 @@
     </row>
     <row r="50" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="70" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B50" s="70" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C50" s="70" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="70" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E50" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F50" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G50" s="70" t="s">
         <v>14</v>
@@ -9783,22 +9786,22 @@
     </row>
     <row r="51" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="70" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B51" s="70" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C51" s="70" t="s">
         <v>19</v>
       </c>
       <c r="D51" s="70" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E51" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F51" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G51" s="70" t="s">
         <v>14</v>
@@ -9813,22 +9816,22 @@
     </row>
     <row r="52" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="70" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B52" s="70" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C52" s="70" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="70" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E52" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F52" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G52" s="70" t="s">
         <v>14</v>
@@ -9843,22 +9846,22 @@
     </row>
     <row r="53" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="70" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B53" s="70" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C53" s="70" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="70" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E53" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F53" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G53" s="70" t="s">
         <v>14</v>
@@ -9873,10 +9876,10 @@
     </row>
     <row r="54" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="70" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B54" s="70" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C54" s="70" t="s">
         <v>8</v>
@@ -9885,10 +9888,10 @@
         <v>14</v>
       </c>
       <c r="E54" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F54" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G54" s="70" t="s">
         <v>14</v>
@@ -9903,10 +9906,10 @@
     </row>
     <row r="55" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="70" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B55" s="70" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C55" s="70" t="s">
         <v>8</v>
@@ -9915,10 +9918,10 @@
         <v>16</v>
       </c>
       <c r="E55" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F55" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G55" s="70" t="s">
         <v>14</v>
@@ -9933,10 +9936,10 @@
     </row>
     <row r="56" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="70" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B56" s="70" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C56" s="70" t="s">
         <v>8</v>
@@ -9945,10 +9948,10 @@
         <v>16</v>
       </c>
       <c r="E56" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F56" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G56" s="70" t="s">
         <v>14</v>
@@ -9963,10 +9966,10 @@
     </row>
     <row r="57" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="70" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C57" s="70" t="s">
         <v>8</v>
@@ -9975,10 +9978,10 @@
         <v>15</v>
       </c>
       <c r="E57" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F57" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G57" s="70" t="s">
         <v>14</v>
@@ -9993,10 +9996,10 @@
     </row>
     <row r="58" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="70" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C58" s="70" t="s">
         <v>8</v>
@@ -10005,10 +10008,10 @@
         <v>16</v>
       </c>
       <c r="E58" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F58" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G58" s="70" t="s">
         <v>14</v>
@@ -10023,22 +10026,22 @@
     </row>
     <row r="59" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="70" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C59" s="70" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="70" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E59" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F59" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G59" s="70" t="s">
         <v>14</v>
@@ -10053,22 +10056,22 @@
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="70" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C60" s="70" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="70" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E60" s="70" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="F60" s="70" t="s">
-        <v>367</v>
+        <v>444</v>
       </c>
       <c r="G60" s="70" t="s">
         <v>14</v>
@@ -10083,10 +10086,10 @@
     </row>
     <row r="61" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B61" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C61" s="71" t="s">
         <v>8</v>
@@ -10095,10 +10098,10 @@
         <v>14</v>
       </c>
       <c r="E61" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F61" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G61" s="71" t="s">
         <v>14</v>
@@ -10113,10 +10116,10 @@
     </row>
     <row r="62" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="71" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B62" s="71" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C62" s="71" t="s">
         <v>13</v>
@@ -10125,10 +10128,10 @@
         <v>16</v>
       </c>
       <c r="E62" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F62" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G62" s="71" t="s">
         <v>14</v>
@@ -10143,10 +10146,10 @@
     </row>
     <row r="63" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="71" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C63" s="71" t="s">
         <v>8</v>
@@ -10155,10 +10158,10 @@
         <v>16</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F63" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G63" s="71" t="s">
         <v>14</v>
@@ -10173,10 +10176,10 @@
     </row>
     <row r="64" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="71" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B64" s="71" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="C64" s="71" t="s">
         <v>8</v>
@@ -10185,10 +10188,10 @@
         <v>15</v>
       </c>
       <c r="E64" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F64" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G64" s="71" t="s">
         <v>14</v>
@@ -10203,10 +10206,10 @@
     </row>
     <row r="65" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="71" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B65" s="71" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C65" s="71" t="s">
         <v>8</v>
@@ -10215,10 +10218,10 @@
         <v>15</v>
       </c>
       <c r="E65" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F65" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G65" s="71" t="s">
         <v>14</v>
@@ -10233,22 +10236,22 @@
     </row>
     <row r="66" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="71" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B66" s="71" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C66" s="71" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="71" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E66" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F66" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G66" s="71" t="s">
         <v>14</v>
@@ -10263,22 +10266,22 @@
     </row>
     <row r="67" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="71" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B67" s="71" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C67" s="71" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="71" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E67" s="71" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F67" s="71" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G67" s="71" t="s">
         <v>14</v>
@@ -10293,10 +10296,10 @@
     </row>
     <row r="68" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B68" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C68" s="72" t="s">
         <v>8</v>
@@ -10305,10 +10308,10 @@
         <v>14</v>
       </c>
       <c r="E68" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F68" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G68" s="72" t="s">
         <v>14</v>
@@ -10323,10 +10326,10 @@
     </row>
     <row r="69" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="72" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B69" s="72" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C69" s="72" t="s">
         <v>13</v>
@@ -10335,10 +10338,10 @@
         <v>16</v>
       </c>
       <c r="E69" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F69" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G69" s="72" t="s">
         <v>14</v>
@@ -10353,10 +10356,10 @@
     </row>
     <row r="70" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="72" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B70" s="72" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C70" s="72" t="s">
         <v>8</v>
@@ -10365,10 +10368,10 @@
         <v>15</v>
       </c>
       <c r="E70" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F70" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G70" s="72" t="s">
         <v>14</v>
@@ -10383,22 +10386,22 @@
     </row>
     <row r="71" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="72" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B71" s="72" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C71" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="72" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E71" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F71" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G71" s="72" t="s">
         <v>14</v>
@@ -10413,22 +10416,22 @@
     </row>
     <row r="72" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="72" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B72" s="72" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C72" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D72" s="72" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="E72" s="72" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F72" s="72" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="G72" s="72" t="s">
         <v>14</v>
@@ -10529,13 +10532,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>344</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
@@ -10873,19 +10876,19 @@
     </row>
     <row r="2" spans="1:12" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="73" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>205</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="F2" s="73" t="s">
         <v>8</v>
@@ -10894,10 +10897,10 @@
         <v>16</v>
       </c>
       <c r="H2" s="73" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="I2" s="73" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J2" s="73" t="s">
         <v>16</v>

</xml_diff>